<commit_message>
model_no_12 and model_no_13 were added.
</commit_message>
<xml_diff>
--- a/model_inspection/model_parameters.xlsx
+++ b/model_inspection/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaanberkeugurlar/Documents/School Lessons/Machine Learning/Project/traffic_signs_recognition/model_inspection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9DCDC4-25B9-8D4F-8FC3-24880C8E11F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0578F0BF-D49A-E74B-8C2D-A7F9B6401F4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="0" windowWidth="20160" windowHeight="21000" xr2:uid="{4622D748-3F4C-5440-89DC-C5F3BAA7A702}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{4622D748-3F4C-5440-89DC-C5F3BAA7A702}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Model No</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>0.0196</t>
+  </si>
+  <si>
+    <t>0.0242</t>
+  </si>
+  <si>
+    <t>0.0236</t>
   </si>
 </sst>
 </file>
@@ -513,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB48003D-A267-FD43-AF47-22F49257954A}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,6 +743,40 @@
         <v>148</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8994859</v>
+      </c>
+      <c r="C13" s="5">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2580523</v>
+      </c>
+      <c r="C14" s="5">
+        <v>9</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="5">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor additions into model parameters.
</commit_message>
<xml_diff>
--- a/model_inspection/model_parameters.xlsx
+++ b/model_inspection/model_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaanberkeugurlar/Documents/School Lessons/Machine Learning/Project/traffic_signs_recognition/model_inspection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0578F0BF-D49A-E74B-8C2D-A7F9B6401F4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA863DD0-20B7-574A-97F8-A1C08FA8A0DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{4622D748-3F4C-5440-89DC-C5F3BAA7A702}"/>
   </bookViews>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB48003D-A267-FD43-AF47-22F49257954A}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>